<commit_message>
Updated with latest estimates
</commit_message>
<xml_diff>
--- a/DS-D files/Static.xlsx
+++ b/DS-D files/Static.xlsx
@@ -16441,10 +16441,10 @@
         </is>
       </c>
       <c r="D669">
-        <v>0</v>
+        <v>2.818060649304283</v>
       </c>
       <c r="E669">
-        <v>92.7141643892343</v>
+        <v>77.11508748397709</v>
       </c>
     </row>
     <row r="670">
@@ -16491,10 +16491,10 @@
         </is>
       </c>
       <c r="D671">
-        <v>2.851496564420309</v>
+        <v>6.214969801346295</v>
       </c>
       <c r="E671">
-        <v>99.37789457481927</v>
+        <v>97.67125372082616</v>
       </c>
     </row>
     <row r="672">
@@ -16514,10 +16514,10 @@
         </is>
       </c>
       <c r="D672">
-        <v>1.341666503691882</v>
+        <v>3.579151351801821</v>
       </c>
       <c r="E672">
-        <v>87.65923877890998</v>
+        <v>77.00568462032463</v>
       </c>
     </row>
     <row r="673">
@@ -16540,7 +16540,7 @@
         <v>0</v>
       </c>
       <c r="E673">
-        <v>67.14151565096333</v>
+        <v>51.51551410311617</v>
       </c>
     </row>
     <row r="674">
@@ -16582,10 +16582,10 @@
         </is>
       </c>
       <c r="D675">
-        <v>3.186580507531383</v>
+        <v>18.80272513372305</v>
       </c>
       <c r="E675">
-        <v>100</v>
+        <v>95.69973602207925</v>
       </c>
     </row>
     <row r="676">
@@ -16605,10 +16605,10 @@
         </is>
       </c>
       <c r="D676">
-        <v>3.023399998011543</v>
+        <v>4.940232790045685</v>
       </c>
       <c r="E676">
-        <v>89.75895633729284</v>
+        <v>86.29492790210902</v>
       </c>
     </row>
     <row r="677">
@@ -16628,10 +16628,10 @@
         </is>
       </c>
       <c r="D677">
-        <v>12.30634354614651</v>
+        <v>23.5340070274588</v>
       </c>
       <c r="E677">
-        <v>100</v>
+        <v>99.5580348881647</v>
       </c>
     </row>
     <row r="678">
@@ -16674,10 +16674,10 @@
         </is>
       </c>
       <c r="D679">
-        <v>24.89120361687245</v>
+        <v>48.45987320770406</v>
       </c>
       <c r="E679">
-        <v>100</v>
+        <v>97.74792125434936</v>
       </c>
     </row>
     <row r="680">
@@ -16697,10 +16697,10 @@
         </is>
       </c>
       <c r="D680">
-        <v>2.399984208275721</v>
+        <v>3.258671848892099</v>
       </c>
       <c r="E680">
-        <v>21.88906280483836</v>
+        <v>19.45088198724385</v>
       </c>
     </row>
     <row r="681">
@@ -16747,10 +16747,10 @@
         </is>
       </c>
       <c r="D682">
-        <v>29.19990596779953</v>
+        <v>51.76696834115641</v>
       </c>
       <c r="E682">
-        <v>100</v>
+        <v>99.33284854808117</v>
       </c>
     </row>
     <row r="683">
@@ -16770,10 +16770,10 @@
         </is>
       </c>
       <c r="D683">
-        <v>1.103534187766827</v>
+        <v>5.32645116992087</v>
       </c>
       <c r="E683">
-        <v>52.84617754774993</v>
+        <v>38.57067583297124</v>
       </c>
     </row>
     <row r="684">
@@ -16793,10 +16793,10 @@
         </is>
       </c>
       <c r="D684">
-        <v>15.71762267974633</v>
+        <v>41.30339991193689</v>
       </c>
       <c r="E684">
-        <v>100</v>
+        <v>87.75981356705135</v>
       </c>
     </row>
     <row r="685">
@@ -16839,10 +16839,10 @@
         </is>
       </c>
       <c r="D686">
-        <v>2.640538819867536</v>
+        <v>3.669690689782173</v>
       </c>
       <c r="E686">
-        <v>97.88791759650852</v>
+        <v>95.58451957564684</v>
       </c>
     </row>
     <row r="687">
@@ -16865,7 +16865,7 @@
         <v>0</v>
       </c>
       <c r="E687">
-        <v>12.93041805199511</v>
+        <v>4.600091855124408</v>
       </c>
     </row>
     <row r="688">
@@ -16888,7 +16888,7 @@
         <v>0</v>
       </c>
       <c r="E688">
-        <v>7.253042831768221</v>
+        <v>5.394627728385085</v>
       </c>
     </row>
     <row r="689">
@@ -16908,10 +16908,10 @@
         </is>
       </c>
       <c r="D689">
-        <v>17.31521632830661</v>
+        <v>27.67852306455712</v>
       </c>
       <c r="E689">
-        <v>100</v>
+        <v>99.1533203837518</v>
       </c>
     </row>
     <row r="690">
@@ -16954,10 +16954,10 @@
         </is>
       </c>
       <c r="D691">
-        <v>0</v>
+        <v>0.3618983406209854</v>
       </c>
       <c r="E691">
-        <v>83.41313778003389</v>
+        <v>55.6224244379651</v>
       </c>
     </row>
     <row r="692">
@@ -16977,10 +16977,10 @@
         </is>
       </c>
       <c r="D692">
-        <v>3.50036387570474</v>
+        <v>14.84082921730442</v>
       </c>
       <c r="E692">
-        <v>84.44092094796846</v>
+        <v>68.97245620203407</v>
       </c>
     </row>
     <row r="693">
@@ -17000,10 +17000,10 @@
         </is>
       </c>
       <c r="D693">
-        <v>11.29664395940612</v>
+        <v>18.79938316501084</v>
       </c>
       <c r="E693">
-        <v>49.83291873006559</v>
+        <v>43.37428371653264</v>
       </c>
     </row>
     <row r="694">
@@ -17023,10 +17023,10 @@
         </is>
       </c>
       <c r="D694">
-        <v>10.69142038241159</v>
+        <v>45.91688908787116</v>
       </c>
       <c r="E694">
-        <v>100</v>
+        <v>91.02804851772109</v>
       </c>
     </row>
     <row r="695">
@@ -17046,10 +17046,10 @@
         </is>
       </c>
       <c r="D695">
-        <v>0</v>
+        <v>2.875622778370469</v>
       </c>
       <c r="E695">
-        <v>61.20778427216141</v>
+        <v>36.95392077248341</v>
       </c>
     </row>
     <row r="696">
@@ -17069,10 +17069,10 @@
         </is>
       </c>
       <c r="D696">
-        <v>21.52017996092467</v>
+        <v>43.99979564942866</v>
       </c>
       <c r="E696">
-        <v>100</v>
+        <v>96.90333295516733</v>
       </c>
     </row>
     <row r="697">
@@ -17092,10 +17092,10 @@
         </is>
       </c>
       <c r="D697">
-        <v>9.034527528829575</v>
+        <v>16.59203973931322</v>
       </c>
       <c r="E697">
-        <v>66.30410486840293</v>
+        <v>64.01675974241402</v>
       </c>
     </row>
     <row r="698">
@@ -19886,10 +19886,10 @@
         </is>
       </c>
       <c r="D814">
-        <v>10.53737554825647</v>
+        <v>21.2269512945991</v>
       </c>
       <c r="E814">
-        <v>93.89512562182524</v>
+        <v>91.9875912620228</v>
       </c>
     </row>
     <row r="815">
@@ -19932,10 +19932,10 @@
         </is>
       </c>
       <c r="D816">
-        <v>0</v>
+        <v>2.78261046459123</v>
       </c>
       <c r="E816">
-        <v>62.82793573896931</v>
+        <v>52.42770943367551</v>
       </c>
     </row>
     <row r="817">
@@ -19955,10 +19955,10 @@
         </is>
       </c>
       <c r="D817">
-        <v>0</v>
+        <v>0.3256097310183747</v>
       </c>
       <c r="E817">
-        <v>26.92452670032845</v>
+        <v>22.45613745420824</v>
       </c>
     </row>
     <row r="818">
@@ -19978,10 +19978,10 @@
         </is>
       </c>
       <c r="D818">
-        <v>0</v>
+        <v>0.4059546626854059</v>
       </c>
       <c r="E818">
-        <v>77.30233450887043</v>
+        <v>71.7078406104323</v>
       </c>
     </row>
     <row r="819">
@@ -20023,10 +20023,10 @@
         </is>
       </c>
       <c r="D820">
-        <v>6.930693069306932</v>
+        <v>16.00621241445315</v>
       </c>
       <c r="E820">
-        <v>95.98774904108824</v>
+        <v>94.22431697750385</v>
       </c>
     </row>
     <row r="821">
@@ -20046,10 +20046,10 @@
         </is>
       </c>
       <c r="D821">
-        <v>5.27366711518392</v>
+        <v>6.70592911681136</v>
       </c>
       <c r="E821">
-        <v>67.00247831227877</v>
+        <v>61.55868370840217</v>
       </c>
     </row>
     <row r="822">
@@ -20069,10 +20069,10 @@
         </is>
       </c>
       <c r="D822">
-        <v>0.6227600157534552</v>
+        <v>3.890319539492073</v>
       </c>
       <c r="E822">
-        <v>83.16555993265102</v>
+        <v>71.36515072692058</v>
       </c>
     </row>
     <row r="823">
@@ -20186,10 +20186,10 @@
         </is>
       </c>
       <c r="D827">
-        <v>51.22844498621063</v>
+        <v>73.07577518868285</v>
       </c>
       <c r="E827">
-        <v>93.64913085386173</v>
+        <v>91.05383239735697</v>
       </c>
     </row>
     <row r="828">
@@ -20209,10 +20209,10 @@
         </is>
       </c>
       <c r="D828">
-        <v>4.305283757338552</v>
+        <v>6.579839820496411</v>
       </c>
       <c r="E828">
-        <v>37.08057800636787</v>
+        <v>29.85936988989425</v>
       </c>
     </row>
     <row r="829">
@@ -20232,10 +20232,10 @@
         </is>
       </c>
       <c r="D829">
-        <v>61.87528127509374</v>
+        <v>67.3671885005934</v>
       </c>
       <c r="E829">
-        <v>100</v>
+        <v>99.04618701183504</v>
       </c>
     </row>
     <row r="830">
@@ -20278,10 +20278,10 @@
         </is>
       </c>
       <c r="D831">
-        <v>2.097358882244741</v>
+        <v>10.07719779551353</v>
       </c>
       <c r="E831">
-        <v>76.9519614396612</v>
+        <v>68.5422885791731</v>
       </c>
     </row>
     <row r="832">
@@ -20304,7 +20304,7 @@
         <v>0</v>
       </c>
       <c r="E832">
-        <v>0.917620906073411</v>
+        <v>0.7602970879352262</v>
       </c>
     </row>
     <row r="833">
@@ -20327,7 +20327,7 @@
         <v>0</v>
       </c>
       <c r="E833">
-        <v>13.89889579381739</v>
+        <v>13.39785699380517</v>
       </c>
     </row>
     <row r="834">
@@ -20347,10 +20347,10 @@
         </is>
       </c>
       <c r="D834">
-        <v>34.98173148137877</v>
+        <v>46.34282331058927</v>
       </c>
       <c r="E834">
-        <v>100</v>
+        <v>99.3620712443515</v>
       </c>
     </row>
     <row r="835">
@@ -20393,10 +20393,10 @@
         </is>
       </c>
       <c r="D836">
-        <v>0.1724473431298865</v>
+        <v>0.3405114414611988</v>
       </c>
       <c r="E836">
-        <v>47.58308157099697</v>
+        <v>41.55262503110227</v>
       </c>
     </row>
     <row r="837">
@@ -20416,10 +20416,10 @@
         </is>
       </c>
       <c r="D837">
-        <v>12.87128712871287</v>
+        <v>22.84944815686427</v>
       </c>
       <c r="E837">
-        <v>96.10594325960263</v>
+        <v>94.59667495168202</v>
       </c>
     </row>
     <row r="838">
@@ -20439,10 +20439,10 @@
         </is>
       </c>
       <c r="D838">
-        <v>20.0078388107727</v>
+        <v>22.48240824770966</v>
       </c>
       <c r="E838">
-        <v>45.61102603852705</v>
+        <v>41.54402398920677</v>
       </c>
     </row>
     <row r="839">
@@ -20506,10 +20506,10 @@
         </is>
       </c>
       <c r="D841">
-        <v>18.52766601456118</v>
+        <v>39.9575375128921</v>
       </c>
       <c r="E841">
-        <v>100</v>
+        <v>99.43213166678704</v>
       </c>
     </row>
     <row r="842">
@@ -20529,10 +20529,10 @@
         </is>
       </c>
       <c r="D842">
-        <v>15.37075395044596</v>
+        <v>21.79574534937334</v>
       </c>
       <c r="E842">
-        <v>84.85960693440168</v>
+        <v>76.76700554708007</v>
       </c>
     </row>
     <row r="843">
@@ -24717,10 +24717,10 @@
         </is>
       </c>
       <c r="D1017">
-        <v>0</v>
+        <v>0.7675438596491228</v>
       </c>
       <c r="E1017">
-        <v>90.04457652303121</v>
+        <v>88.12842825916609</v>
       </c>
     </row>
     <row r="1018">
@@ -24763,7 +24763,7 @@
         </is>
       </c>
       <c r="D1019">
-        <v>1.204819277108434</v>
+        <v>4.451038575667656</v>
       </c>
       <c r="E1019">
         <v>91.78198850329998</v>
@@ -24786,7 +24786,7 @@
         </is>
       </c>
       <c r="D1020">
-        <v>0</v>
+        <v>0.5649717514124294</v>
       </c>
       <c r="E1020">
         <v>46.08792846497764</v>
@@ -24809,7 +24809,7 @@
         </is>
       </c>
       <c r="D1021">
-        <v>0</v>
+        <v>0.3891050583657588</v>
       </c>
       <c r="E1021">
         <v>17.61083743842365</v>
@@ -24854,7 +24854,7 @@
         </is>
       </c>
       <c r="D1023">
-        <v>0</v>
+        <v>1.193576388888889</v>
       </c>
       <c r="E1023">
         <v>86.93966864645202</v>
@@ -24877,10 +24877,10 @@
         </is>
       </c>
       <c r="D1024">
-        <v>10</v>
+        <v>21.54471544715447</v>
       </c>
       <c r="E1024">
-        <v>99.58734525447042</v>
+        <v>95.17878234725652</v>
       </c>
     </row>
     <row r="1025">
@@ -24900,10 +24900,10 @@
         </is>
       </c>
       <c r="D1025">
-        <v>2.352941176470588</v>
+        <v>9.495548961424333</v>
       </c>
       <c r="E1025">
-        <v>98.35521769177609</v>
+        <v>97.55560145975349</v>
       </c>
     </row>
     <row r="1026">
@@ -25036,10 +25036,10 @@
         </is>
       </c>
       <c r="D1031">
-        <v>1.063829787234043</v>
+        <v>2.390581253439901</v>
       </c>
       <c r="E1031">
-        <v>55.23850085178875</v>
+        <v>45.97910291401318</v>
       </c>
     </row>
     <row r="1032">
@@ -25059,10 +25059,10 @@
         </is>
       </c>
       <c r="D1032">
-        <v>13.13868613138686</v>
+        <v>20</v>
       </c>
       <c r="E1032">
-        <v>94.11764705882352</v>
+        <v>77.36185383244207</v>
       </c>
     </row>
     <row r="1033">
@@ -25105,7 +25105,7 @@
         </is>
       </c>
       <c r="D1034">
-        <v>0</v>
+        <v>3.560830860534125</v>
       </c>
       <c r="E1034">
         <v>95.11858735218975</v>
@@ -25175,7 +25175,7 @@
         <v>25.35712932439089</v>
       </c>
       <c r="E1037">
-        <v>100</v>
+        <v>98.51632047477746</v>
       </c>
     </row>
     <row r="1038">
@@ -25218,10 +25218,10 @@
         </is>
       </c>
       <c r="D1039">
-        <v>0</v>
+        <v>0.525866035627424</v>
       </c>
       <c r="E1039">
-        <v>83.29238329238329</v>
+        <v>73.82960162838035</v>
       </c>
     </row>
     <row r="1040">
@@ -25241,10 +25241,10 @@
         </is>
       </c>
       <c r="D1040">
-        <v>31.50684931506849</v>
+        <v>40.5940594059406</v>
       </c>
       <c r="E1040">
-        <v>100</v>
+        <v>96.67194928684627</v>
       </c>
     </row>
     <row r="1041">
@@ -25264,7 +25264,7 @@
         </is>
       </c>
       <c r="D1041">
-        <v>1.012373498574955</v>
+        <v>3.264095074875772</v>
       </c>
       <c r="E1041">
         <v>33.4447582715691</v>
@@ -25331,10 +25331,10 @@
         </is>
       </c>
       <c r="D1044">
-        <v>7.894736842105263</v>
+        <v>41.07373868046572</v>
       </c>
       <c r="E1044">
-        <v>100</v>
+        <v>98.15270935960592</v>
       </c>
     </row>
     <row r="1045">
@@ -25354,10 +25354,10 @@
         </is>
       </c>
       <c r="D1045">
-        <v>0</v>
+        <v>4.616347905282332</v>
       </c>
       <c r="E1045">
-        <v>60.88235294117646</v>
+        <v>39.0625</v>
       </c>
     </row>
     <row r="1046">

</xml_diff>